<commit_message>
Added ability to generate report for each architecture on separate sheet.
</commit_message>
<xml_diff>
--- a/src/main/resources/com/jernejerin/Measurements_template.xlsx
+++ b/src/main/resources/com/jernejerin/Measurements_template.xlsx
@@ -7,9 +7,9 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" calcOnSave="0"/>
 </workbook>
 </file>
 

</xml_diff>